<commit_message>
Weer Bug fixes het houd niet op xD
</commit_message>
<xml_diff>
--- a/Developing/Bug Report.xlsx
+++ b/Developing/Bug Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="65">
   <si>
     <t>Bug nr.</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Paraaf: Fahrettin</t>
+  </si>
+  <si>
+    <t>Paraaf: Sven</t>
+  </si>
+  <si>
+    <t>Sven</t>
+  </si>
+  <si>
+    <t>Paraaf:</t>
   </si>
 </sst>
 </file>
@@ -675,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="P65" sqref="P65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +912,7 @@
       <c r="C10" s="12"/>
       <c r="O10" s="2"/>
       <c r="P10" s="3" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="Q10" s="7"/>
     </row>
@@ -969,7 +978,7 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1032,10 +1041,10 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="9"/>
+      <c r="B23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="12"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>

</xml_diff>